<commit_message>
Trabalho completo - falta revisao geral
</commit_message>
<xml_diff>
--- a/Exemplos.xlsx
+++ b/Exemplos.xlsx
@@ -5,16 +5,17 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\OneDrive\IME-BMAC\7o Sem - 01_2019\MAP2040 - TC\Trabalho final\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/912a6e5d1950f402/IME-BMAC/7o Sem - 01_2019/MAP2040 - TC/Trabalho final/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="128" documentId="8_{D43E324D-7FD5-4CE2-B8C3-1C8A46FCB0FE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{29735999-1C2C-4DF2-AC3D-3F559EB6047F}"/>
+  <xr:revisionPtr revIDLastSave="147" documentId="8_{D43E324D-7FD5-4CE2-B8C3-1C8A46FCB0FE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{004D1204-72BD-47E4-8693-6094A319279F}"/>
   <bookViews>
-    <workbookView xWindow="828" yWindow="-108" windowWidth="22320" windowHeight="13176" activeTab="1" xr2:uid="{FB307AB7-987C-437D-853F-245A386BDE3E}"/>
+    <workbookView xWindow="828" yWindow="-108" windowWidth="22320" windowHeight="13176" activeTab="2" xr2:uid="{FB307AB7-987C-437D-853F-245A386BDE3E}"/>
   </bookViews>
   <sheets>
     <sheet name="Roleta" sheetId="1" r:id="rId1"/>
     <sheet name="Crossover" sheetId="2" r:id="rId2"/>
+    <sheet name="Ising" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -86,7 +87,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -115,8 +116,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="18"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -135,8 +143,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="10">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -239,12 +259,27 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="1" tint="0.249977111117893"/>
+      </left>
+      <right style="thin">
+        <color theme="1" tint="0.249977111117893"/>
+      </right>
+      <top style="thin">
+        <color theme="1" tint="0.249977111117893"/>
+      </top>
+      <bottom style="thin">
+        <color theme="1" tint="0.249977111117893"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -274,6 +309,10 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1688,8 +1727,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0ECD9A74-A884-478F-9045-55D933348156}">
   <dimension ref="B2:R34"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A22" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A28" sqref="A28:S34"/>
+    <sheetView showGridLines="0" topLeftCell="A22" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H45" sqref="H45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2401,4 +2440,285 @@
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B11692C1-21BA-4822-B300-72558E69B265}">
+  <dimension ref="A1:M78"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:L12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="1.6640625" customWidth="1"/>
+    <col min="2" max="11" width="4.33203125" customWidth="1"/>
+    <col min="12" max="12" width="1.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" ht="23.4" x14ac:dyDescent="0.45">
+      <c r="A1" s="19"/>
+      <c r="B1" s="19"/>
+      <c r="C1" s="19"/>
+      <c r="D1" s="19"/>
+      <c r="E1" s="19"/>
+      <c r="F1" s="19"/>
+      <c r="G1" s="19"/>
+      <c r="H1" s="19"/>
+      <c r="I1" s="19"/>
+      <c r="J1" s="19"/>
+      <c r="K1" s="19"/>
+      <c r="L1" s="19"/>
+      <c r="M1" s="19"/>
+    </row>
+    <row r="2" spans="1:13" ht="23.4" x14ac:dyDescent="0.45">
+      <c r="A2" s="19"/>
+      <c r="B2" s="20"/>
+      <c r="C2" s="20"/>
+      <c r="D2" s="20"/>
+      <c r="E2" s="20"/>
+      <c r="F2" s="20"/>
+      <c r="G2" s="20"/>
+      <c r="H2" s="20"/>
+      <c r="I2" s="20"/>
+      <c r="J2" s="20"/>
+      <c r="K2" s="20"/>
+      <c r="L2" s="19"/>
+      <c r="M2" s="19"/>
+    </row>
+    <row r="3" spans="1:13" ht="23.4" x14ac:dyDescent="0.45">
+      <c r="A3" s="19"/>
+      <c r="B3" s="20"/>
+      <c r="C3" s="20"/>
+      <c r="D3" s="20"/>
+      <c r="E3" s="20"/>
+      <c r="F3" s="20"/>
+      <c r="G3" s="20"/>
+      <c r="H3" s="20"/>
+      <c r="I3" s="20"/>
+      <c r="J3" s="20"/>
+      <c r="K3" s="20"/>
+      <c r="L3" s="19"/>
+      <c r="M3" s="19"/>
+    </row>
+    <row r="4" spans="1:13" ht="23.4" x14ac:dyDescent="0.45">
+      <c r="A4" s="19"/>
+      <c r="B4" s="20"/>
+      <c r="C4" s="20"/>
+      <c r="D4" s="20"/>
+      <c r="E4" s="20"/>
+      <c r="F4" s="20"/>
+      <c r="G4" s="20"/>
+      <c r="H4" s="20"/>
+      <c r="I4" s="20"/>
+      <c r="J4" s="20"/>
+      <c r="K4" s="20"/>
+      <c r="L4" s="19"/>
+      <c r="M4" s="19"/>
+    </row>
+    <row r="5" spans="1:13" ht="23.4" x14ac:dyDescent="0.45">
+      <c r="A5" s="19"/>
+      <c r="B5" s="20"/>
+      <c r="C5" s="20"/>
+      <c r="D5" s="20"/>
+      <c r="E5" s="20"/>
+      <c r="F5" s="20"/>
+      <c r="G5" s="20"/>
+      <c r="H5" s="20"/>
+      <c r="I5" s="20"/>
+      <c r="J5" s="20"/>
+      <c r="K5" s="20"/>
+      <c r="L5" s="19"/>
+      <c r="M5" s="19"/>
+    </row>
+    <row r="6" spans="1:13" ht="23.4" x14ac:dyDescent="0.45">
+      <c r="A6" s="19"/>
+      <c r="B6" s="20"/>
+      <c r="C6" s="20"/>
+      <c r="D6" s="20"/>
+      <c r="E6" s="20"/>
+      <c r="F6" s="20"/>
+      <c r="G6" s="20"/>
+      <c r="H6" s="20"/>
+      <c r="I6" s="20"/>
+      <c r="J6" s="20"/>
+      <c r="K6" s="20"/>
+      <c r="L6" s="19"/>
+      <c r="M6" s="19"/>
+    </row>
+    <row r="7" spans="1:13" ht="23.4" x14ac:dyDescent="0.45">
+      <c r="A7" s="19"/>
+      <c r="B7" s="20"/>
+      <c r="C7" s="20"/>
+      <c r="D7" s="20"/>
+      <c r="E7" s="20"/>
+      <c r="F7" s="20"/>
+      <c r="G7" s="20"/>
+      <c r="H7" s="20"/>
+      <c r="I7" s="20"/>
+      <c r="J7" s="20"/>
+      <c r="K7" s="20"/>
+      <c r="L7" s="19"/>
+      <c r="M7" s="19"/>
+    </row>
+    <row r="8" spans="1:13" ht="23.4" x14ac:dyDescent="0.45">
+      <c r="A8" s="19"/>
+      <c r="B8" s="21"/>
+      <c r="C8" s="21"/>
+      <c r="D8" s="21"/>
+      <c r="E8" s="21"/>
+      <c r="F8" s="22"/>
+      <c r="G8" s="22"/>
+      <c r="H8" s="22"/>
+      <c r="I8" s="22"/>
+      <c r="J8" s="22"/>
+      <c r="K8" s="22"/>
+      <c r="L8" s="19"/>
+      <c r="M8" s="19"/>
+    </row>
+    <row r="9" spans="1:13" ht="23.4" x14ac:dyDescent="0.45">
+      <c r="A9" s="19"/>
+      <c r="B9" s="21"/>
+      <c r="C9" s="21"/>
+      <c r="D9" s="21"/>
+      <c r="E9" s="21"/>
+      <c r="F9" s="22"/>
+      <c r="G9" s="22"/>
+      <c r="H9" s="22"/>
+      <c r="I9" s="22"/>
+      <c r="J9" s="22"/>
+      <c r="K9" s="22"/>
+      <c r="L9" s="19"/>
+      <c r="M9" s="19"/>
+    </row>
+    <row r="10" spans="1:13" ht="23.4" x14ac:dyDescent="0.45">
+      <c r="A10" s="19"/>
+      <c r="B10" s="21"/>
+      <c r="C10" s="21"/>
+      <c r="D10" s="21"/>
+      <c r="E10" s="21"/>
+      <c r="F10" s="22"/>
+      <c r="G10" s="22"/>
+      <c r="H10" s="22"/>
+      <c r="I10" s="22"/>
+      <c r="J10" s="22"/>
+      <c r="K10" s="22"/>
+      <c r="L10" s="19"/>
+      <c r="M10" s="19"/>
+    </row>
+    <row r="11" spans="1:13" ht="23.4" x14ac:dyDescent="0.45">
+      <c r="A11" s="19"/>
+      <c r="B11" s="21"/>
+      <c r="C11" s="21"/>
+      <c r="D11" s="21"/>
+      <c r="E11" s="21"/>
+      <c r="F11" s="22"/>
+      <c r="G11" s="22"/>
+      <c r="H11" s="22"/>
+      <c r="I11" s="22"/>
+      <c r="J11" s="22"/>
+      <c r="K11" s="22"/>
+      <c r="L11" s="19"/>
+      <c r="M11" s="19"/>
+    </row>
+    <row r="12" spans="1:13" ht="23.4" x14ac:dyDescent="0.45">
+      <c r="A12" s="19"/>
+      <c r="B12" s="19"/>
+      <c r="C12" s="19"/>
+      <c r="D12" s="19"/>
+      <c r="E12" s="19"/>
+      <c r="F12" s="19"/>
+      <c r="G12" s="19"/>
+      <c r="H12" s="19"/>
+      <c r="I12" s="19"/>
+      <c r="J12" s="19"/>
+      <c r="K12" s="19"/>
+      <c r="L12" s="19"/>
+      <c r="M12" s="19"/>
+    </row>
+    <row r="13" spans="1:13" ht="23.4" x14ac:dyDescent="0.45">
+      <c r="A13" s="19"/>
+      <c r="B13" s="19"/>
+      <c r="C13" s="19"/>
+      <c r="D13" s="19"/>
+      <c r="E13" s="19"/>
+      <c r="F13" s="19"/>
+      <c r="G13" s="19"/>
+      <c r="H13" s="19"/>
+      <c r="I13" s="19"/>
+      <c r="J13" s="19"/>
+      <c r="K13" s="19"/>
+      <c r="L13" s="19"/>
+      <c r="M13" s="19"/>
+    </row>
+    <row r="14" spans="1:13" s="19" customFormat="1" ht="23.4" x14ac:dyDescent="0.45"/>
+    <row r="15" spans="1:13" s="19" customFormat="1" ht="23.4" x14ac:dyDescent="0.45"/>
+    <row r="16" spans="1:13" s="19" customFormat="1" ht="23.4" x14ac:dyDescent="0.45"/>
+    <row r="17" s="19" customFormat="1" ht="23.4" x14ac:dyDescent="0.45"/>
+    <row r="18" s="19" customFormat="1" ht="23.4" x14ac:dyDescent="0.45"/>
+    <row r="19" s="19" customFormat="1" ht="23.4" x14ac:dyDescent="0.45"/>
+    <row r="20" s="19" customFormat="1" ht="23.4" x14ac:dyDescent="0.45"/>
+    <row r="21" s="19" customFormat="1" ht="23.4" x14ac:dyDescent="0.45"/>
+    <row r="22" s="19" customFormat="1" ht="23.4" x14ac:dyDescent="0.45"/>
+    <row r="23" s="19" customFormat="1" ht="23.4" x14ac:dyDescent="0.45"/>
+    <row r="24" s="19" customFormat="1" ht="23.4" x14ac:dyDescent="0.45"/>
+    <row r="25" s="19" customFormat="1" ht="23.4" x14ac:dyDescent="0.45"/>
+    <row r="26" s="19" customFormat="1" ht="23.4" x14ac:dyDescent="0.45"/>
+    <row r="27" s="19" customFormat="1" ht="23.4" x14ac:dyDescent="0.45"/>
+    <row r="28" s="19" customFormat="1" ht="23.4" x14ac:dyDescent="0.45"/>
+    <row r="29" s="19" customFormat="1" ht="23.4" x14ac:dyDescent="0.45"/>
+    <row r="30" s="19" customFormat="1" ht="23.4" x14ac:dyDescent="0.45"/>
+    <row r="31" s="19" customFormat="1" ht="23.4" x14ac:dyDescent="0.45"/>
+    <row r="32" s="19" customFormat="1" ht="23.4" x14ac:dyDescent="0.45"/>
+    <row r="33" s="19" customFormat="1" ht="23.4" x14ac:dyDescent="0.45"/>
+    <row r="34" s="19" customFormat="1" ht="23.4" x14ac:dyDescent="0.45"/>
+    <row r="35" s="19" customFormat="1" ht="23.4" x14ac:dyDescent="0.45"/>
+    <row r="36" s="19" customFormat="1" ht="23.4" x14ac:dyDescent="0.45"/>
+    <row r="37" s="19" customFormat="1" ht="23.4" x14ac:dyDescent="0.45"/>
+    <row r="38" s="19" customFormat="1" ht="23.4" x14ac:dyDescent="0.45"/>
+    <row r="39" s="19" customFormat="1" ht="23.4" x14ac:dyDescent="0.45"/>
+    <row r="40" s="19" customFormat="1" ht="23.4" x14ac:dyDescent="0.45"/>
+    <row r="41" s="19" customFormat="1" ht="23.4" x14ac:dyDescent="0.45"/>
+    <row r="42" s="19" customFormat="1" ht="23.4" x14ac:dyDescent="0.45"/>
+    <row r="43" s="19" customFormat="1" ht="23.4" x14ac:dyDescent="0.45"/>
+    <row r="44" s="19" customFormat="1" ht="23.4" x14ac:dyDescent="0.45"/>
+    <row r="45" s="19" customFormat="1" ht="23.4" x14ac:dyDescent="0.45"/>
+    <row r="46" s="19" customFormat="1" ht="23.4" x14ac:dyDescent="0.45"/>
+    <row r="47" s="19" customFormat="1" ht="23.4" x14ac:dyDescent="0.45"/>
+    <row r="48" s="19" customFormat="1" ht="23.4" x14ac:dyDescent="0.45"/>
+    <row r="49" s="19" customFormat="1" ht="23.4" x14ac:dyDescent="0.45"/>
+    <row r="50" s="19" customFormat="1" ht="23.4" x14ac:dyDescent="0.45"/>
+    <row r="51" s="19" customFormat="1" ht="23.4" x14ac:dyDescent="0.45"/>
+    <row r="52" s="19" customFormat="1" ht="23.4" x14ac:dyDescent="0.45"/>
+    <row r="53" s="19" customFormat="1" ht="23.4" x14ac:dyDescent="0.45"/>
+    <row r="54" s="19" customFormat="1" ht="23.4" x14ac:dyDescent="0.45"/>
+    <row r="55" s="19" customFormat="1" ht="23.4" x14ac:dyDescent="0.45"/>
+    <row r="56" s="19" customFormat="1" ht="23.4" x14ac:dyDescent="0.45"/>
+    <row r="57" s="19" customFormat="1" ht="23.4" x14ac:dyDescent="0.45"/>
+    <row r="58" s="19" customFormat="1" ht="23.4" x14ac:dyDescent="0.45"/>
+    <row r="59" s="19" customFormat="1" ht="23.4" x14ac:dyDescent="0.45"/>
+    <row r="60" s="19" customFormat="1" ht="23.4" x14ac:dyDescent="0.45"/>
+    <row r="61" s="19" customFormat="1" ht="23.4" x14ac:dyDescent="0.45"/>
+    <row r="62" s="19" customFormat="1" ht="23.4" x14ac:dyDescent="0.45"/>
+    <row r="63" s="19" customFormat="1" ht="23.4" x14ac:dyDescent="0.45"/>
+    <row r="64" s="19" customFormat="1" ht="23.4" x14ac:dyDescent="0.45"/>
+    <row r="65" s="19" customFormat="1" ht="23.4" x14ac:dyDescent="0.45"/>
+    <row r="66" s="19" customFormat="1" ht="23.4" x14ac:dyDescent="0.45"/>
+    <row r="67" s="19" customFormat="1" ht="23.4" x14ac:dyDescent="0.45"/>
+    <row r="68" s="19" customFormat="1" ht="23.4" x14ac:dyDescent="0.45"/>
+    <row r="69" s="19" customFormat="1" ht="23.4" x14ac:dyDescent="0.45"/>
+    <row r="70" s="19" customFormat="1" ht="23.4" x14ac:dyDescent="0.45"/>
+    <row r="71" s="19" customFormat="1" ht="23.4" x14ac:dyDescent="0.45"/>
+    <row r="72" s="19" customFormat="1" ht="23.4" x14ac:dyDescent="0.45"/>
+    <row r="73" s="19" customFormat="1" ht="23.4" x14ac:dyDescent="0.45"/>
+    <row r="74" s="19" customFormat="1" ht="23.4" x14ac:dyDescent="0.45"/>
+    <row r="75" s="19" customFormat="1" ht="23.4" x14ac:dyDescent="0.45"/>
+    <row r="76" s="19" customFormat="1" ht="23.4" x14ac:dyDescent="0.45"/>
+    <row r="77" s="19" customFormat="1" ht="23.4" x14ac:dyDescent="0.45"/>
+    <row r="78" s="19" customFormat="1" ht="23.4" x14ac:dyDescent="0.45"/>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>